<commit_message>
modify for interval & last
</commit_message>
<xml_diff>
--- a/emgForEA/special_case.xlsx
+++ b/emgForEA/special_case.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ergolab2\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FTP\EMG-Analysis\emgForEA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>A003</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -39,6 +39,18 @@
   </si>
   <si>
     <t>A003</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TASK1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A006</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -377,10 +389,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -407,6 +419,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>